<commit_message>
Compared FEC an FX option to xVA Lite
</commit_message>
<xml_diff>
--- a/excel_file/FEC_atm_vol_surface.xlsx
+++ b/excel_file/FEC_atm_vol_surface.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\stochastic_process_calibration_2022\excel_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42DC32CF-5C3C-4A63-8326-FD2F03EE1FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68050B8-3189-43CD-88E9-58D5B42BAB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FC99AD29-4392-4706-887A-2ED290A18A63}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="constant_vol_surface" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -504,7 +504,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -531,7 +531,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
-        <f ca="1">1/12</f>
+        <f>1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="B3" s="2">
@@ -540,7 +540,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
-        <f ca="1">2/12</f>
+        <f>2/12</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="B4" s="2">
@@ -549,7 +549,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
-        <f ca="1">3/12</f>
+        <f>3/12</f>
         <v>0.25</v>
       </c>
       <c r="B5" s="2">
@@ -558,7 +558,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
-        <f ca="1">6/12</f>
+        <f>6/12</f>
         <v>0.5</v>
       </c>
       <c r="B6" s="2">
@@ -567,7 +567,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
-        <f ca="1">9/12</f>
+        <f>9/12</f>
         <v>0.75</v>
       </c>
       <c r="B7" s="2">
@@ -576,7 +576,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
-        <f ca="1">1</f>
+        <f>1</f>
         <v>1</v>
       </c>
       <c r="B8" s="2">

</xml_diff>